<commit_message>
Implement spreadsheet provider models (#43)
* Renames connectors folder to providers

* Creates spreadsheet provider models

* Renames bank related attributes

* Adds pydantic dependency

* Creates custom data type for dates

* Uses AuroraDate type on Payment model date

* Merge with main

* Uses CNABDate type on Payment date attribute

* Adds enum for registration type

* Updates registration type enum definition

* Updates Tipo de Inscriçao da Empresa to use CNPJ instead of a number

* Adds unit tests for spreadsheet provider models
</commit_message>
<xml_diff>
--- a/sample/spreadsheet_sample.xlsx
+++ b/sample/spreadsheet_sample.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Empresa" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="59">
   <si>
     <t xml:space="preserve">* Nome da Empresa</t>
   </si>
@@ -78,7 +78,7 @@
     <t xml:space="preserve"> Vinta Servicos e Solucoes Tec</t>
   </si>
   <si>
-    <t xml:space="preserve">9</t>
+    <t xml:space="preserve">CNPJ</t>
   </si>
   <si>
     <t xml:space="preserve">99999999000999</t>
@@ -91,6 +91,9 @@
   </si>
   <si>
     <t xml:space="preserve">1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9</t>
   </si>
   <si>
     <t xml:space="preserve">999999</t>
@@ -457,13 +460,13 @@
   </sheetPr>
   <dimension ref="A1:AA2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
+      <selection pane="bottomLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="33.71"/>
@@ -564,37 +567,37 @@
         <v>22</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="H2" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="I2" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="I2" s="6" t="s">
-        <v>18</v>
-      </c>
       <c r="J2" s="6" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="K2" s="7" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="L2" s="7" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="M2" s="7" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="N2" s="7" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="O2" s="7" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="P2" s="7" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="Q2" s="7" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -615,13 +618,13 @@
   </sheetPr>
   <dimension ref="A1:AB1000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="33.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="32.57"/>
@@ -643,19 +646,19 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>6</v>
@@ -667,19 +670,19 @@
         <v>8</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="J1" s="3" t="s">
         <v>10</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="L1" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="M1" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="N1" s="3" t="s">
         <v>13</v>
@@ -707,55 +710,55 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D2" s="6" t="s">
         <v>21</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="J2" s="7" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="K2" s="7" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="L2" s="7" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="M2" s="7" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="N2" s="7" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="O2" s="7" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="P2" s="7" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="Q2" s="7" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19744,7 +19747,7 @@
       <selection pane="bottomLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="34.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="20.3"/>
@@ -19754,28 +19757,28 @@
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B2" s="5"/>
       <c r="C2" s="5" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Fix spreadsheet registration type and identification number
</commit_message>
<xml_diff>
--- a/sample/spreadsheet_sample.xlsx
+++ b/sample/spreadsheet_sample.xlsx
@@ -78,7 +78,7 @@
     <t xml:space="preserve"> Vinta Servicos e Solucoes Tec</t>
   </si>
   <si>
-    <t xml:space="preserve">CNPJ</t>
+    <t xml:space="preserve">CGC/CNPJ</t>
   </si>
   <si>
     <t xml:space="preserve">99999999000999</t>
@@ -463,10 +463,10 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="bottomLeft" activeCell="C20" activeCellId="0" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.515625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="33.71"/>
@@ -624,7 +624,7 @@
       <selection pane="bottomLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="33.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="32.57"/>
@@ -19744,10 +19744,10 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
+      <selection pane="bottomLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="34.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="20.3"/>

</xml_diff>

<commit_message>
Implement CNAB conversion to fixed-width file (#10)
* Implement payroll get_CNAB file

* Implement CNAB as fixed width

* Update CnabFile to take in list of batches and upate registration number default

* Fix spreadsheet registration type and identification number

* Add ignore unsubscriptable-object
</commit_message>
<xml_diff>
--- a/sample/spreadsheet_sample.xlsx
+++ b/sample/spreadsheet_sample.xlsx
@@ -78,7 +78,7 @@
     <t xml:space="preserve"> Vinta Servicos e Solucoes Tec</t>
   </si>
   <si>
-    <t xml:space="preserve">CNPJ</t>
+    <t xml:space="preserve">CGC/CNPJ</t>
   </si>
   <si>
     <t xml:space="preserve">99999999000999</t>
@@ -463,10 +463,10 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="bottomLeft" activeCell="C20" activeCellId="0" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.515625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="33.71"/>
@@ -624,7 +624,7 @@
       <selection pane="bottomLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="33.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="32.57"/>
@@ -19744,10 +19744,10 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
+      <selection pane="bottomLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="34.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="20.3"/>

</xml_diff>